<commit_message>
Breadcrumbs broke need to find out why
</commit_message>
<xml_diff>
--- a/Docs/Test Cases.xlsx
+++ b/Docs/Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okechi\Desktop\Javascript\Projects\STLC Example Project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68B8E22-E53E-4820-A292-B4D0F8B4C5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F630E2-E6BC-4BC9-A47D-08C56004F81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6390" yWindow="720" windowWidth="23835" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23700" yWindow="0" windowWidth="14700" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,13 +517,6 @@
 2. Choose a sub-category from the categories on the top banner (Women, Men etc...).
 3. Verify that the page is correct.
 4. Choose a product.
-5. Verify the product information (name, price, options).</t>
-  </si>
-  <si>
-    <t>1. Navigate to "https://magento.softwaretestingboard.com/".
-2. Choose a sub-category from the categories on the top banner (Women, Men etc...).
-3. Verify that the page is correct.
-4. Choose a product.
 5. Click on the breadcrumbs trail.
 6. Verify the user is take back to the correct page.</t>
   </si>
@@ -784,6 +777,13 @@
   </si>
   <si>
     <t>Successfully purchased a product without an account</t>
+  </si>
+  <si>
+    <t>1. Navigate to "https://magento.softwaretestingboard.com/".
+2. Navigate to a sub-category.
+3. Verify that the page is correct.
+4. Choose a product.
+5. Verify the product information (name, price, options).</t>
   </si>
 </sst>
 </file>
@@ -891,7 +891,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1188,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,7 +1404,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1419,10 +1419,10 @@
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="3" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -1440,10 +1440,10 @@
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -1461,10 +1461,10 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1482,10 +1482,10 @@
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -1503,10 +1503,10 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="225" x14ac:dyDescent="0.25">
@@ -1524,10 +1524,10 @@
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="180" x14ac:dyDescent="0.25">
@@ -1547,10 +1547,10 @@
         <v>78</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -1568,10 +1568,10 @@
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -1589,10 +1589,10 @@
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -1610,10 +1610,10 @@
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="225" x14ac:dyDescent="0.25">
@@ -1631,10 +1631,10 @@
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="225" x14ac:dyDescent="0.25">
@@ -1652,10 +1652,10 @@
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -1673,10 +1673,10 @@
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -1694,10 +1694,10 @@
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1714,13 +1714,13 @@
         <v>73</v>
       </c>
       <c r="E24" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -1731,19 +1731,19 @@
         <v>62</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E25" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1760,13 +1760,13 @@
         <v>73</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="180" x14ac:dyDescent="0.25">
@@ -1783,13 +1783,13 @@
         <v>72</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -1806,13 +1806,13 @@
         <v>73</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="180" x14ac:dyDescent="0.25">
@@ -1829,13 +1829,13 @@
         <v>73</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="195" x14ac:dyDescent="0.25">
@@ -1852,13 +1852,13 @@
         <v>72</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -1875,13 +1875,13 @@
         <v>72</v>
       </c>
       <c r="E31" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="225" x14ac:dyDescent="0.25">
@@ -1898,13 +1898,13 @@
         <v>72</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="240" x14ac:dyDescent="0.25">
@@ -1921,13 +1921,13 @@
         <v>72</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="225" x14ac:dyDescent="0.25">
@@ -1938,17 +1938,17 @@
         <v>71</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>72</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>